<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T05:39:57.876Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,40 +449,40 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C2" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D2" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E2" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G2">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
-        <v>00:30</v>
+        <v>08:00</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>Less Spicy</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,37 +493,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 22:51</v>
+        <v>2026-01-14 17:08</v>
       </c>
       <c r="C3" t="str">
-        <v>Ketki</v>
+        <v>Mrunal</v>
       </c>
       <c r="D3" t="str">
-        <v>1608</v>
+        <v>KLV B 2108</v>
       </c>
       <c r="E3" t="str">
-        <v>3159135521</v>
+        <v>9404665203</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Wheat Chapati x40</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>16:51</v>
+        <v>00:30</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,25 +537,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C4" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D4" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E4" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F4" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,13 +564,13 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L4" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -581,13 +581,13 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C5" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D5" t="str">
         <v>420</v>
@@ -596,10 +596,10 @@
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,13 +608,13 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L5" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C6" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D6" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E6" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,10 +652,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,16 +669,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C7" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E7" t="str">
         <v>7588930329</v>
@@ -690,16 +690,16 @@
         <v>15</v>
       </c>
       <c r="H7" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K7" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,37 +713,37 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C8" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D8" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E8" t="str">
         <v>7588930329</v>
       </c>
       <c r="F8" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H8" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K8" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C9" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D9" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E9" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -784,10 +784,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K9" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,16 +801,16 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C10" t="str">
         <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E10" t="str">
         <v>9096648553</v>
@@ -828,10 +828,10 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K10" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C11" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E11" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F11" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -872,10 +872,10 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K11" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C12" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D12" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E12" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F12" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G12">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -919,7 +919,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K12" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C13" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D13" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E13" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F13" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H13" t="str">
         <v>NEW</v>
@@ -960,10 +960,10 @@
         <v>PENDING</v>
       </c>
       <c r="J13" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K13" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,25 +977,25 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C14" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D14" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E14" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F14" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G14">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H14" t="str">
         <v>NEW</v>
@@ -1007,7 +1007,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K14" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L14" t="str">
         <v/>
@@ -1021,58 +1021,102 @@
     </row>
     <row r="15">
       <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D15" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I15" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J15" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K15" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B16" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C16" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D16" t="str">
         <v>B 304</v>
       </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
-      <c r="F15" t="str">
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>30</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H16" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I15" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J15" t="str">
+      <c r="I16" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J16" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K15" t="str">
+      <c r="K16" t="str">
         <v>16:45</v>
       </c>
-      <c r="L15" t="str">
-        <v/>
-      </c>
-      <c r="M15" t="str">
-        <v/>
-      </c>
-      <c r="N15" t="str">
+      <c r="L16" t="str">
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N16"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1102,53 +1146,76 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-19</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="F2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>600</v>
+      </c>
+      <c r="F3">
+        <v>600</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>340</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T05:41:04.937Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,10 +449,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C2" t="str">
         <v>Prajakta Patil</v>
@@ -476,13 +476,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
       </c>
       <c r="L2" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -493,40 +493,40 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C3" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D3" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E3" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G3">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H3" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K3" t="str">
-        <v>00:30</v>
+        <v>08:00</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>Less Spicy</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -537,37 +537,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 22:51</v>
+        <v>2026-01-14 17:08</v>
       </c>
       <c r="C4" t="str">
-        <v>Ketki</v>
+        <v>Mrunal</v>
       </c>
       <c r="D4" t="str">
-        <v>1608</v>
+        <v>KLV B 2108</v>
       </c>
       <c r="E4" t="str">
-        <v>3159135521</v>
+        <v>9404665203</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Wheat Chapati x40</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>16:51</v>
+        <v>00:30</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C5" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D5" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E5" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F5" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,13 +608,13 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L5" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M5" t="str">
         <v/>
@@ -625,13 +625,13 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C6" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D6" t="str">
         <v>420</v>
@@ -640,10 +640,10 @@
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,13 +652,13 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K6" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L6" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C7" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D7" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E7" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,10 +696,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,16 +713,16 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C8" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D8" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E8" t="str">
         <v>7588930329</v>
@@ -734,16 +734,16 @@
         <v>15</v>
       </c>
       <c r="H8" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K8" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,37 +757,37 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C9" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D9" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E9" t="str">
         <v>7588930329</v>
       </c>
       <c r="F9" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H9" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I9" t="str">
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K9" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D10" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E10" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -828,10 +828,10 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K10" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,16 +845,16 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C11" t="str">
         <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E11" t="str">
         <v>9096648553</v>
@@ -872,10 +872,10 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K11" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C12" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D12" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E12" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F12" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -916,10 +916,10 @@
         <v>PENDING</v>
       </c>
       <c r="J12" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K12" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C13" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D13" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E13" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F13" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G13">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H13" t="str">
         <v>NEW</v>
@@ -963,7 +963,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K13" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,25 +977,25 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C14" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D14" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E14" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F14" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H14" t="str">
         <v>NEW</v>
@@ -1004,10 +1004,10 @@
         <v>PENDING</v>
       </c>
       <c r="J14" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K14" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L14" t="str">
         <v/>
@@ -1021,25 +1021,25 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C15" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D15" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E15" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F15" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H15" t="str">
         <v>NEW</v>
@@ -1051,7 +1051,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K15" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L15" t="str">
         <v/>
@@ -1065,51 +1065,95 @@
     </row>
     <row r="16">
       <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D16" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I16" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J16" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K16" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
         <v>1</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B17" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C17" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D17" t="str">
         <v>B 304</v>
       </c>
-      <c r="E16" t="str">
-        <v/>
-      </c>
-      <c r="F16" t="str">
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>30</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H17" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I16" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J16" t="str">
+      <c r="I17" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J17" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K16" t="str">
+      <c r="K17" t="str">
         <v>16:45</v>
       </c>
-      <c r="L16" t="str">
-        <v/>
-      </c>
-      <c r="M16" t="str">
-        <v/>
-      </c>
-      <c r="N16" t="str">
+      <c r="L17" t="str">
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N17"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1149,7 +1193,7 @@
         <v>2026-01-19</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1158,13 +1202,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>105</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T05:42:03.561Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,10 +449,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C2" t="str">
         <v>Prajakta Patil</v>
@@ -464,10 +464,10 @@
         <v>779868817</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G2">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,7 +476,7 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C3" t="str">
         <v>Prajakta Patil</v>
@@ -520,13 +520,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K3" t="str">
         <v>08:00</v>
       </c>
       <c r="L3" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -537,40 +537,40 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C4" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D4" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E4" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G4">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H4" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K4" t="str">
-        <v>00:30</v>
+        <v>08:00</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>Less Spicy</v>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -581,37 +581,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 22:51</v>
+        <v>2026-01-14 17:08</v>
       </c>
       <c r="C5" t="str">
-        <v>Ketki</v>
+        <v>Mrunal</v>
       </c>
       <c r="D5" t="str">
-        <v>1608</v>
+        <v>KLV B 2108</v>
       </c>
       <c r="E5" t="str">
-        <v>3159135521</v>
+        <v>9404665203</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Wheat Chapati x40</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="H5" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I5" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>16:51</v>
+        <v>00:30</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C6" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D6" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F6" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -652,13 +652,13 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L6" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M6" t="str">
         <v/>
@@ -669,13 +669,13 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C7" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D7" t="str">
         <v>420</v>
@@ -684,10 +684,10 @@
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,13 +696,13 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K7" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L7" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C8" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D8" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E8" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,10 +740,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K8" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,16 +757,16 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C9" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D9" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E9" t="str">
         <v>7588930329</v>
@@ -778,16 +778,16 @@
         <v>15</v>
       </c>
       <c r="H9" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I9" t="str">
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K9" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,37 +801,37 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C10" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D10" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E10" t="str">
         <v>7588930329</v>
       </c>
       <c r="F10" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I10" t="str">
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K10" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C11" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D11" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E11" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F11" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -872,10 +872,10 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K11" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,16 +889,16 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C12" t="str">
         <v>Pooja</v>
       </c>
       <c r="D12" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E12" t="str">
         <v>9096648553</v>
@@ -916,10 +916,10 @@
         <v>PENDING</v>
       </c>
       <c r="J12" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K12" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C13" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D13" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E13" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F13" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H13" t="str">
         <v>NEW</v>
@@ -960,10 +960,10 @@
         <v>PENDING</v>
       </c>
       <c r="J13" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K13" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,25 +977,25 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C14" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D14" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E14" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F14" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G14">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H14" t="str">
         <v>NEW</v>
@@ -1007,7 +1007,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K14" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L14" t="str">
         <v/>
@@ -1021,25 +1021,25 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C15" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D15" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E15" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F15" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H15" t="str">
         <v>NEW</v>
@@ -1048,10 +1048,10 @@
         <v>PENDING</v>
       </c>
       <c r="J15" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K15" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L15" t="str">
         <v/>
@@ -1065,25 +1065,25 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C16" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D16" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E16" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F16" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G16">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H16" t="str">
         <v>NEW</v>
@@ -1095,7 +1095,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K16" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L16" t="str">
         <v/>
@@ -1109,51 +1109,95 @@
     </row>
     <row r="17">
       <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D17" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I17" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J17" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K17" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L17" t="str">
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
         <v>1</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B18" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C18" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D18" t="str">
         <v>B 304</v>
       </c>
-      <c r="E17" t="str">
-        <v/>
-      </c>
-      <c r="F17" t="str">
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>30</v>
       </c>
-      <c r="H17" t="str">
+      <c r="H18" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I17" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J17" t="str">
+      <c r="I18" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J18" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K17" t="str">
+      <c r="K18" t="str">
         <v>16:45</v>
       </c>
-      <c r="L17" t="str">
-        <v/>
-      </c>
-      <c r="M17" t="str">
-        <v/>
-      </c>
-      <c r="N17" t="str">
+      <c r="L18" t="str">
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N18"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1193,7 +1237,7 @@
         <v>2026-01-19</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1202,13 +1246,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>210</v>
+        <v>285</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>210</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T08:37:40.360Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C2" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D2" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E2" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x3</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,7 +476,7 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K2" t="str">
         <v>08:00</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C3" t="str">
         <v>Prajakta Patil</v>
@@ -508,10 +508,10 @@
         <v>779868817</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G3">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,7 +520,7 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K3" t="str">
         <v>08:00</v>
@@ -537,10 +537,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C4" t="str">
         <v>Prajakta Patil</v>
@@ -564,13 +564,13 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K4" t="str">
         <v>08:00</v>
       </c>
       <c r="L4" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -581,40 +581,40 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-14 17:08</v>
+        <v>2026-01-19 05:39</v>
       </c>
       <c r="C5" t="str">
-        <v>Mrunal</v>
+        <v>Prajakta Patil</v>
       </c>
       <c r="D5" t="str">
-        <v>KLV B 2108</v>
+        <v>A 804</v>
       </c>
       <c r="E5" t="str">
-        <v>9404665203</v>
+        <v>779868817</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x40</v>
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
       </c>
       <c r="G5">
-        <v>600</v>
+        <v>105</v>
       </c>
       <c r="H5" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K5" t="str">
-        <v>00:30</v>
+        <v>08:00</v>
       </c>
       <c r="L5" t="str">
-        <v/>
+        <v>Less Spicy</v>
       </c>
       <c r="M5" t="str">
         <v/>
@@ -625,37 +625,37 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 22:51</v>
+        <v>2026-01-14 17:08</v>
       </c>
       <c r="C6" t="str">
-        <v>Ketki</v>
+        <v>Mrunal</v>
       </c>
       <c r="D6" t="str">
-        <v>1608</v>
+        <v>KLV B 2108</v>
       </c>
       <c r="E6" t="str">
-        <v>3159135521</v>
+        <v>9404665203</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Wheat Chapati x40</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="H6" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I6" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K6" t="str">
-        <v>16:51</v>
+        <v>00:30</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C7" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D7" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E7" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F7" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -696,13 +696,13 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L7" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M7" t="str">
         <v/>
@@ -713,13 +713,13 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C8" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D8" t="str">
         <v>420</v>
@@ -728,10 +728,10 @@
         <v/>
       </c>
       <c r="F8" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,13 +740,13 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K8" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L8" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M8" t="str">
         <v/>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C9" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D9" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E9" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -784,10 +784,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K9" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,16 +801,16 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C10" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D10" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E10" t="str">
         <v>7588930329</v>
@@ -822,16 +822,16 @@
         <v>15</v>
       </c>
       <c r="H10" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I10" t="str">
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K10" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,37 +845,37 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C11" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D11" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E11" t="str">
         <v>7588930329</v>
       </c>
       <c r="F11" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H11" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I11" t="str">
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K11" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C12" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D12" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E12" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F12" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -916,10 +916,10 @@
         <v>PENDING</v>
       </c>
       <c r="J12" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K12" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,16 +933,16 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C13" t="str">
         <v>Pooja</v>
       </c>
       <c r="D13" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E13" t="str">
         <v>9096648553</v>
@@ -960,10 +960,10 @@
         <v>PENDING</v>
       </c>
       <c r="J13" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K13" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,25 +977,25 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C14" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D14" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E14" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F14" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H14" t="str">
         <v>NEW</v>
@@ -1004,10 +1004,10 @@
         <v>PENDING</v>
       </c>
       <c r="J14" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K14" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L14" t="str">
         <v/>
@@ -1021,25 +1021,25 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C15" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D15" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E15" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F15" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G15">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H15" t="str">
         <v>NEW</v>
@@ -1051,7 +1051,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K15" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L15" t="str">
         <v/>
@@ -1065,25 +1065,25 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C16" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D16" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E16" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F16" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G16">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H16" t="str">
         <v>NEW</v>
@@ -1092,10 +1092,10 @@
         <v>PENDING</v>
       </c>
       <c r="J16" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K16" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L16" t="str">
         <v/>
@@ -1109,25 +1109,25 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C17" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D17" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E17" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F17" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G17">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H17" t="str">
         <v>NEW</v>
@@ -1139,7 +1139,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K17" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L17" t="str">
         <v/>
@@ -1153,51 +1153,95 @@
     </row>
     <row r="18">
       <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D18" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I18" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J18" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K18" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L18" t="str">
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
         <v>1</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B19" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C19" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D19" t="str">
         <v>B 304</v>
       </c>
-      <c r="E18" t="str">
-        <v/>
-      </c>
-      <c r="F18" t="str">
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H18" t="str">
+      <c r="H19" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I18" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J18" t="str">
+      <c r="I19" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J19" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K18" t="str">
+      <c r="K19" t="str">
         <v>16:45</v>
       </c>
-      <c r="L18" t="str">
-        <v/>
-      </c>
-      <c r="M18" t="str">
-        <v/>
-      </c>
-      <c r="N18" t="str">
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N19"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1237,7 +1281,7 @@
         <v>2026-01-19</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1246,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>285</v>
+        <v>375</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>285</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T08:59:50.219Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -734,7 +734,7 @@
         <v>50</v>
       </c>
       <c r="H8" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
@@ -749,7 +749,7 @@
         <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M8" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N8" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>340</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T08:59:58.291Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="H9" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I9" t="str">
         <v>PENDING</v>
@@ -793,7 +793,7 @@
         <v/>
       </c>
       <c r="M9" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N9" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>290</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:00:37.739Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -1086,7 +1086,7 @@
         <v>60</v>
       </c>
       <c r="H16" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I16" t="str">
         <v>PENDING</v>
@@ -1101,7 +1101,7 @@
         <v/>
       </c>
       <c r="M16" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N16" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>260</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:00:52.777Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -1130,7 +1130,7 @@
         <v>30</v>
       </c>
       <c r="H17" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I17" t="str">
         <v>PENDING</v>
@@ -1145,7 +1145,7 @@
         <v/>
       </c>
       <c r="M17" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N17" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>200</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:00:56.399Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -1174,7 +1174,7 @@
         <v>15</v>
       </c>
       <c r="H18" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I18" t="str">
         <v>PENDING</v>
@@ -1189,7 +1189,7 @@
         <v/>
       </c>
       <c r="M18" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N18" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:00.731Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -1218,7 +1218,7 @@
         <v>30</v>
       </c>
       <c r="H19" t="str">
-        <v>COOKING</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I19" t="str">
         <v>PENDING</v>
@@ -1233,7 +1233,7 @@
         <v/>
       </c>
       <c r="M19" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N19" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>155</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:22.802Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -822,7 +822,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I10" t="str">
         <v>PENDING</v>
@@ -837,7 +837,7 @@
         <v/>
       </c>
       <c r="M10" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N10" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:26.332Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -954,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I13" t="str">
         <v>PENDING</v>
@@ -969,7 +969,7 @@
         <v/>
       </c>
       <c r="M13" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N13" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:32.960Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -998,7 +998,7 @@
         <v>15</v>
       </c>
       <c r="H14" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I14" t="str">
         <v>PENDING</v>
@@ -1013,7 +1013,7 @@
         <v/>
       </c>
       <c r="M14" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N14" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:37.714Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -1042,7 +1042,7 @@
         <v>30</v>
       </c>
       <c r="H15" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I15" t="str">
         <v>PENDING</v>
@@ -1057,7 +1057,7 @@
         <v/>
       </c>
       <c r="M15" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N15" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:53.300Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -690,7 +690,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
@@ -705,7 +705,7 @@
         <v/>
       </c>
       <c r="M7" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N7" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:01:56.882Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="H12" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I12" t="str">
         <v>PENDING</v>
@@ -925,7 +925,7 @@
         <v/>
       </c>
       <c r="M12" t="str">
-        <v/>
+        <v>test order</v>
       </c>
       <c r="N12" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:13:03.553Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -866,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="str">
-        <v>NEW</v>
+        <v>CANCELLED</v>
       </c>
       <c r="I11" t="str">
         <v>PENDING</v>
@@ -881,7 +881,7 @@
         <v/>
       </c>
       <c r="M11" t="str">
-        <v/>
+        <v>test</v>
       </c>
       <c r="N11" t="str">
         <v/>
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:13:43.959Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -464,10 +464,10 @@
         <v>9967195227</v>
       </c>
       <c r="F2" t="str">
-        <v>Pohe x3</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>375</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:18:43.662Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -470,10 +470,10 @@
         <v>120</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-18</v>
@@ -756,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -765,10 +765,10 @@
         <v>525</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G2">
-        <v>525</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:18:48.129Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -514,10 +514,10 @@
         <v>120</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-20</v>
@@ -756,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -765,10 +765,10 @@
         <v>525</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="G2">
-        <v>405</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-19.xlsx - 2026-01-19T09:19:19.381Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-19.xlsx
@@ -514,7 +514,7 @@
         <v>120</v>
       </c>
       <c r="H3" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PAID</v>
@@ -756,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>